<commit_message>
Correct invalid times, replace "." with ":"
</commit_message>
<xml_diff>
--- a/timetables/stansted.xlsx
+++ b/timetables/stansted.xlsx
@@ -17,54 +17,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="4">
   <si>
-    <t>Stansted</t>
+    <t>London Stansted Airport</t>
   </si>
   <si>
-    <t>Stratford</t>
+    <t>London Stratford</t>
   </si>
   <si>
-    <t>Liverpool Street</t>
+    <t>London Liverpool Street</t>
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>14.30</t>
-  </si>
-  <si>
-    <t>15.55</t>
-  </si>
-  <si>
-    <t>16.25</t>
-  </si>
-  <si>
-    <t>17.55</t>
-  </si>
-  <si>
-    <t>21.25</t>
-  </si>
-  <si>
-    <t>21.30</t>
-  </si>
-  <si>
-    <t>22.25</t>
-  </si>
-  <si>
-    <t>23.30</t>
-  </si>
-  <si>
-    <t>10.25</t>
-  </si>
-  <si>
-    <t>18.55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="hh:mm"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11.0"/>
@@ -140,8 +113,8 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -646,8 +619,8 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="5" t="s">
-        <v>4</v>
+      <c r="A26" s="5">
+        <v>0.6041666666666666</v>
       </c>
       <c r="B26" s="2">
         <v>0.642361111111111</v>
@@ -660,8 +633,8 @@
       <c r="A27" s="2">
         <v>0.625</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>5</v>
+      <c r="B27" s="5">
+        <v>0.6631944444444444</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>3</v>
@@ -671,8 +644,8 @@
       <c r="A28" s="2">
         <v>0.6458333333333334</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>6</v>
+      <c r="B28" s="5">
+        <v>0.6840277777777778</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>3</v>
@@ -704,8 +677,8 @@
       <c r="A31" s="2">
         <v>0.7083333333333334</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>7</v>
+      <c r="B31" s="5">
+        <v>0.7465277777777778</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>3</v>
@@ -781,8 +754,8 @@
       <c r="A38" s="2">
         <v>0.8541666666666666</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>8</v>
+      <c r="B38" s="5">
+        <v>0.8923611111111112</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>3</v>
@@ -800,11 +773,11 @@
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>10</v>
+      <c r="A40" s="5">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0.9340277777777778</v>
       </c>
       <c r="C40" s="2">
         <v>0.9444444444444445</v>
@@ -844,8 +817,8 @@
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="5" t="s">
-        <v>11</v>
+      <c r="A44" s="5">
+        <v>0.9791666666666666</v>
       </c>
       <c r="B44" s="2">
         <v>0.010416666666666666</v>
@@ -5816,8 +5789,8 @@
       <c r="B15" s="2">
         <v>0.3993055555555556</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>12</v>
+      <c r="C15" s="5">
+        <v>0.4340277777777778</v>
       </c>
     </row>
     <row r="16">
@@ -5989,8 +5962,8 @@
       <c r="A31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="2">
-        <v>0.7326388888888888</v>
+      <c r="B31" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C31" s="2">
         <v>0.7673611111111112</v>
@@ -6003,8 +5976,8 @@
       <c r="B32" s="2">
         <v>0.7534722222222222</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>13</v>
+      <c r="C32" s="5">
+        <v>0.7881944444444444</v>
       </c>
     </row>
     <row r="33">

</xml_diff>